<commit_message>
EPBDS-11024 add more tests for Smartlookup table should not be transposed during compilation
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11024_Transposed_Tables.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-11024_Transposed_Tables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\demo\openl-demo\user-workspace\DEFAULT\SmartLookupBug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\openl-repo\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB6BDE2-A8EC-4C63-B2CE-C8B7C9A89758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2A7197-21DE-44AC-8046-50D49FB22D7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="690" windowWidth="23700" windowHeight="15060" xr2:uid="{13F5640C-D687-48A5-897F-53CA4E0E44F2}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="17025" windowHeight="13290" xr2:uid="{13F5640C-D687-48A5-897F-53CA4E0E44F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>AL</t>
   </si>
@@ -77,21 +77,41 @@
     <t>Cov1</t>
   </si>
   <si>
-    <t>SmartLookup String[] CoveredOptionValueListCodes (  String param1,  String  param2, String param3, int param4,String  param5)</t>
-  </si>
-  <si>
-    <t>SmartLookup String[] test(  String param1,  String  param2, String param3, int param4,String  param5)</t>
-  </si>
-  <si>
     <t>SmartLookup String test(  String param1,  String  param2, String param3, int param4,String  param5)</t>
+  </si>
+  <si>
+    <t>SmartLookup  Integer mySmartLookup(String  carNum, CarValue carValue , Double param3, Double param4)</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>pam</t>
+  </si>
+  <si>
+    <t>50.0</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>Datatype CarValue &lt;String&gt;</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>SmartLookup  Integer mySmartLookupTrans(String  carNum, CarValue carValue , Double param3, Double param4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,7 +128,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -151,13 +171,6 @@
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -174,7 +187,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442" rgb="5B9BD5"/>
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor rgb="FFDBE5F1"/>
       </patternFill>
     </fill>
@@ -191,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -358,13 +371,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -422,11 +483,24 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{4A1B3E51-277B-47C4-93DB-2A3CAB4186DF}"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{B8BB6E99-A644-4899-9DB1-48BBF992E9B9}"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{4A1B3E51-277B-47C4-93DB-2A3CAB4186DF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -442,9 +516,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -482,7 +556,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -588,7 +662,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -738,17 +812,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBE75930-ADBD-4FAD-B3F7-1AE2CBDB54B1}">
-  <dimension ref="C6:W11"/>
+  <dimension ref="C6:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="6" spans="3:23" ht="15.75">
       <c r="C6" s="15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -966,8 +1040,154 @@
       <c r="V11" s="13"/>
       <c r="W11" s="14"/>
     </row>
+    <row r="16" spans="3:23">
+      <c r="C16" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="3:6">
+      <c r="C17" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="C18" s="21"/>
+      <c r="D18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6">
+      <c r="C19" s="24">
+        <v>3</v>
+      </c>
+      <c r="D19" s="24">
+        <v>2</v>
+      </c>
+      <c r="E19" s="24">
+        <v>3</v>
+      </c>
+      <c r="F19" s="24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="C20" s="24">
+        <v>45</v>
+      </c>
+      <c r="D20" s="24">
+        <v>2</v>
+      </c>
+      <c r="E20" s="24">
+        <v>1</v>
+      </c>
+      <c r="F20" s="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6">
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6">
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="3:6">
+      <c r="C25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6">
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6">
+      <c r="C28" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" spans="3:6">
+      <c r="C29" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="24">
+        <v>3</v>
+      </c>
+      <c r="F29" s="24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6">
+      <c r="C30" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="24">
+        <v>2</v>
+      </c>
+      <c r="F30" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6">
+      <c r="C31" s="23"/>
+      <c r="D31" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="24">
+        <v>3</v>
+      </c>
+      <c r="F31" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:6">
+      <c r="C32" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="24">
+        <v>7</v>
+      </c>
+      <c r="E32" s="24">
+        <v>3</v>
+      </c>
+      <c r="F32" s="24">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="15">
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:D29"/>
     <mergeCell ref="J9:W9"/>
     <mergeCell ref="J10:W10"/>
     <mergeCell ref="J11:W11"/>

</xml_diff>